<commit_message>
added viaf id through benedict
</commit_message>
<xml_diff>
--- a/authorities_to_be_added.xlsx
+++ b/authorities_to_be_added.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="154" documentId="5_{3427F915-78A8-4E76-BB1C-A0C5BDAB3C9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C0E4F629-59E4-4534-940F-76F4361B851C}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="5_{3427F915-78A8-4E76-BB1C-A0C5BDAB3C9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{579CE532-8B41-43C2-AADF-78DED544D687}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
   <si>
     <t>Name</t>
   </si>
@@ -446,6 +446,210 @@
   </si>
   <si>
     <t>http://viaf.org/viaf/2806841</t>
+  </si>
+  <si>
+    <t>Oliver, Pedro Juan</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/34607051</t>
+  </si>
+  <si>
+    <t>Gronovius, Abraham</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/61677396</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/12384559</t>
+  </si>
+  <si>
+    <t>Barbier, Jules</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/86596074</t>
+  </si>
+  <si>
+    <t>Bardili, Guilielmus Henricus</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/49966518</t>
+  </si>
+  <si>
+    <t>Staveren, Augustinus van</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/89208065</t>
+  </si>
+  <si>
+    <t>Bleyswick, Francois van</t>
+  </si>
+  <si>
+    <t>Baret, Eugene</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/36964332</t>
+  </si>
+  <si>
+    <t>Barker, Edmund Henry</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/39716436</t>
+  </si>
+  <si>
+    <t>Baron, Augustus</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/7193500</t>
+  </si>
+  <si>
+    <t>Barreau, H.</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/7691155044886272520003</t>
+  </si>
+  <si>
+    <t>Peronne, Joseph-Max</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/61854282</t>
+  </si>
+  <si>
+    <t>Ecalle, Pierre Felix</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/56646541</t>
+  </si>
+  <si>
+    <t>Charpentier, Jean-Pierre</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/22274769</t>
+  </si>
+  <si>
+    <t>Vincent, C.J.B.J.</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/121850838</t>
+  </si>
+  <si>
+    <t>Barth, Friedrich Gottlieb</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/908603</t>
+  </si>
+  <si>
+    <t>Vinet, Elie</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/27100990</t>
+  </si>
+  <si>
+    <t>Accorso, Mariangelo</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/42899404</t>
+  </si>
+  <si>
+    <t>Rivinus, Andreas</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/40246385</t>
+  </si>
+  <si>
+    <t>Schrijver, Pieter</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/24732263</t>
+  </si>
+  <si>
+    <t>Baumstark, Anton</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/59164719</t>
+  </si>
+  <si>
+    <t>Baune, Jaques de la</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/39454999</t>
+  </si>
+  <si>
+    <t>Baxter, William</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/5266955</t>
+  </si>
+  <si>
+    <t>Becher, Christian</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/42743606</t>
+  </si>
+  <si>
+    <t>Becher, Friedrich Liebgott</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/49657969</t>
+  </si>
+  <si>
+    <t>Beck, Charles</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/37658375</t>
+  </si>
+  <si>
+    <t>Beck, Christian Daniel</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/57357633</t>
+  </si>
+  <si>
+    <t>Becker, Gustavus</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/42580693</t>
+  </si>
+  <si>
+    <t>Becker, Ulrich Justus Heinrich</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/25344923</t>
+  </si>
+  <si>
+    <t>Becker, William Adolf</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/88728074</t>
+  </si>
+  <si>
+    <t>Beesly, A.H.</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/29898952</t>
+  </si>
+  <si>
+    <t>Beger, Laurentius</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/56907766</t>
+  </si>
+  <si>
+    <t>Beier, Karl</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/444806</t>
+  </si>
+  <si>
+    <t>Benecke, Karl</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/263942005</t>
+  </si>
+  <si>
+    <t>Benedict, Traugott Friedrich</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/12739365</t>
   </si>
 </sst>
 </file>
@@ -811,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1392,6 +1596,278 @@
         <v>141</v>
       </c>
     </row>
+    <row r="72" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="33.6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:B50">
     <sortCondition ref="A28"/>
@@ -1401,8 +1877,9 @@
     <hyperlink ref="B15" r:id="rId2" xr:uid="{3625D120-5336-46D5-AE4B-E63BEB4D0114}"/>
     <hyperlink ref="B21" r:id="rId3" xr:uid="{4C6FD6DD-1109-40A5-9AEB-9AD2973FEFFF}"/>
     <hyperlink ref="B29" r:id="rId4" xr:uid="{48E39569-CD60-4443-BBD7-D862D41D02BD}"/>
+    <hyperlink ref="B104" r:id="rId5" xr:uid="{2BDBBDF5-F4AC-45CC-9608-2522D53484B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cleaned up anthologies and added work ids for all of Virgil
</commit_message>
<xml_diff>
--- a/authorities_to_be_added.xlsx
+++ b/authorities_to_be_added.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="225" documentId="5_{3427F915-78A8-4E76-BB1C-A0C5BDAB3C9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{579CE532-8B41-43C2-AADF-78DED544D687}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FEB5E7-707B-422B-8E52-56534826335C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
   <si>
     <t>Name</t>
   </si>
@@ -650,6 +650,18 @@
   </si>
   <si>
     <t>http://viaf.org/viaf/12739365</t>
+  </si>
+  <si>
+    <t>Oberthur, Franz</t>
+  </si>
+  <si>
+    <t>Mai, Angelo</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/79150290</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/100180720</t>
   </si>
 </sst>
 </file>
@@ -1015,20 +1027,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.21875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="44.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1036,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1044,7 +1056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1052,7 +1064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1068,7 +1080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1076,7 +1088,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1084,7 +1096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1092,7 +1104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1100,7 +1112,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1108,7 +1120,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1116,7 +1128,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1124,7 +1136,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1132,7 +1144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1140,7 +1152,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1148,7 +1160,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1156,7 +1168,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -1164,7 +1176,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -1172,7 +1184,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -1180,7 +1192,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -1188,7 +1200,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>70</v>
       </c>
@@ -1196,7 +1208,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>74</v>
       </c>
@@ -1204,7 +1216,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -1212,7 +1224,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -1220,7 +1232,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -1228,7 +1240,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
@@ -1236,7 +1248,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>86</v>
       </c>
@@ -1244,7 +1256,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
@@ -1252,7 +1264,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>90</v>
       </c>
@@ -1260,7 +1272,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -1268,7 +1280,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -1276,7 +1288,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>96</v>
       </c>
@@ -1284,7 +1296,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>98</v>
       </c>
@@ -1292,7 +1304,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
@@ -1300,7 +1312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -1308,7 +1320,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1316,7 +1328,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
@@ -1324,7 +1336,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -1332,7 +1344,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
@@ -1340,7 +1352,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -1348,7 +1360,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
@@ -1356,7 +1368,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
@@ -1364,7 +1376,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -1372,7 +1384,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
@@ -1380,7 +1392,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1388,7 +1400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>66</v>
       </c>
@@ -1396,7 +1408,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>32</v>
       </c>
@@ -1404,7 +1416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1412,7 +1424,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
@@ -1420,7 +1432,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>84</v>
       </c>
@@ -1428,7 +1440,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
@@ -1444,7 +1456,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
@@ -1452,7 +1464,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
@@ -1460,7 +1472,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>108</v>
       </c>
@@ -1468,7 +1480,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>110</v>
       </c>
@@ -1476,7 +1488,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
@@ -1484,7 +1496,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>114</v>
       </c>
@@ -1492,7 +1504,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
@@ -1500,7 +1512,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>118</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
@@ -1516,7 +1528,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
@@ -1524,7 +1536,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
@@ -1532,7 +1544,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
@@ -1540,7 +1552,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>129</v>
       </c>
@@ -1548,7 +1560,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
@@ -1556,7 +1568,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>132</v>
       </c>
@@ -1564,7 +1576,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>135</v>
       </c>
@@ -1572,7 +1584,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
@@ -1580,7 +1592,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>138</v>
       </c>
@@ -1588,7 +1600,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>140</v>
       </c>
@@ -1596,7 +1608,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
@@ -1604,7 +1616,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>144</v>
       </c>
@@ -1612,7 +1624,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>153</v>
       </c>
@@ -1620,7 +1632,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>147</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>149</v>
       </c>
@@ -1636,7 +1648,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>151</v>
       </c>
@@ -1644,7 +1656,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>154</v>
       </c>
@@ -1652,7 +1664,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>156</v>
       </c>
@@ -1660,7 +1672,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>158</v>
       </c>
@@ -1668,7 +1680,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="33.6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>160</v>
       </c>
@@ -1676,7 +1688,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
@@ -1684,7 +1696,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>164</v>
       </c>
@@ -1692,7 +1704,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>166</v>
       </c>
@@ -1700,7 +1712,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>168</v>
       </c>
@@ -1708,7 +1720,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>170</v>
       </c>
@@ -1716,7 +1728,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>172</v>
       </c>
@@ -1724,7 +1736,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>174</v>
       </c>
@@ -1732,7 +1744,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>176</v>
       </c>
@@ -1740,7 +1752,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>178</v>
       </c>
@@ -1748,7 +1760,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>180</v>
       </c>
@@ -1756,7 +1768,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>182</v>
       </c>
@@ -1764,7 +1776,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>184</v>
       </c>
@@ -1772,7 +1784,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>186</v>
       </c>
@@ -1780,7 +1792,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>188</v>
       </c>
@@ -1788,7 +1800,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>190</v>
       </c>
@@ -1796,7 +1808,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>192</v>
       </c>
@@ -1804,7 +1816,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>194</v>
       </c>
@@ -1812,7 +1824,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>196</v>
       </c>
@@ -1820,7 +1832,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>198</v>
       </c>
@@ -1828,7 +1840,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>200</v>
       </c>
@@ -1836,7 +1848,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>202</v>
       </c>
@@ -1844,7 +1856,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>204</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>206</v>
       </c>
@@ -1860,12 +1872,28 @@
         <v>207</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added work id's for Lucan, Minucius F, Manilius, Curtius Rufus
</commit_message>
<xml_diff>
--- a/authorities_to_be_added.xlsx
+++ b/authorities_to_be_added.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="329" documentId="5_{3427F915-78A8-4E76-BB1C-A0C5BDAB3C9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9B76F2D1-F265-4771-B9A9-FA40DD94C6E6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49ABC9D5-B2D0-487F-9CD8-49FE9CE5E6C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="308">
   <si>
     <t>Name</t>
   </si>
@@ -941,6 +941,9 @@
   </si>
   <si>
     <t>http://viaf.org/viaf/59826654</t>
+  </si>
+  <si>
+    <t>Angelo Mai</t>
   </si>
 </sst>
 </file>
@@ -1306,20 +1309,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.21875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="44.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1351,7 +1354,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1367,7 +1370,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1399,7 +1402,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1423,7 +1426,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1431,7 +1434,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1447,7 +1450,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -1455,7 +1458,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -1463,7 +1466,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -1471,7 +1474,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -1479,7 +1482,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>70</v>
       </c>
@@ -1487,7 +1490,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>74</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -1511,7 +1514,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -1519,7 +1522,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
@@ -1527,7 +1530,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>86</v>
       </c>
@@ -1535,7 +1538,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>90</v>
       </c>
@@ -1551,7 +1554,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -1567,7 +1570,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>96</v>
       </c>
@@ -1575,7 +1578,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>98</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
@@ -1591,7 +1594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
@@ -1615,7 +1618,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
@@ -1631,7 +1634,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
@@ -1647,7 +1650,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
@@ -1655,7 +1658,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
@@ -1671,7 +1674,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>66</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>32</v>
       </c>
@@ -1695,7 +1698,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1703,7 +1706,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>84</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1727,7 +1730,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
@@ -1735,7 +1738,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
@@ -1743,7 +1746,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
@@ -1751,7 +1754,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>108</v>
       </c>
@@ -1759,7 +1762,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>110</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>114</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>118</v>
       </c>
@@ -1799,7 +1802,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>129</v>
       </c>
@@ -1839,7 +1842,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>132</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>135</v>
       </c>
@@ -1863,7 +1866,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>138</v>
       </c>
@@ -1879,7 +1882,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>140</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>144</v>
       </c>
@@ -1903,7 +1906,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>153</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>147</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>149</v>
       </c>
@@ -1927,7 +1930,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>151</v>
       </c>
@@ -1935,7 +1938,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>154</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>156</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>158</v>
       </c>
@@ -1959,7 +1962,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="33.6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>160</v>
       </c>
@@ -1967,7 +1970,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>164</v>
       </c>
@@ -1983,7 +1986,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>166</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>168</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>170</v>
       </c>
@@ -2007,7 +2010,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>172</v>
       </c>
@@ -2015,7 +2018,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>174</v>
       </c>
@@ -2023,7 +2026,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>176</v>
       </c>
@@ -2031,7 +2034,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>178</v>
       </c>
@@ -2039,7 +2042,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>180</v>
       </c>
@@ -2047,7 +2050,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>182</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>184</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>186</v>
       </c>
@@ -2071,7 +2074,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>188</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>190</v>
       </c>
@@ -2087,7 +2090,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>192</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>194</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>196</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>198</v>
       </c>
@@ -2119,7 +2122,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>200</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>202</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>204</v>
       </c>
@@ -2143,7 +2146,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>206</v>
       </c>
@@ -2151,7 +2154,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>208</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>210</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>212</v>
       </c>
@@ -2175,7 +2178,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>214</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>216</v>
       </c>
@@ -2191,7 +2194,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>218</v>
       </c>
@@ -2199,7 +2202,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>220</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>222</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>224</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>226</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>228</v>
       </c>
@@ -2239,7 +2242,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>230</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>232</v>
       </c>
@@ -2255,7 +2258,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>234</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>236</v>
       </c>
@@ -2271,7 +2274,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>238</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>240</v>
       </c>
@@ -2287,7 +2290,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>242</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>244</v>
       </c>
@@ -2303,7 +2306,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>246</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>248</v>
       </c>
@@ -2319,7 +2322,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>250</v>
       </c>
@@ -2327,7 +2330,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>257</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>253</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>255</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>258</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>260</v>
       </c>
@@ -2367,7 +2370,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>262</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>263</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>266</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>268</v>
       </c>
@@ -2399,7 +2402,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>270</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>272</v>
       </c>
@@ -2415,7 +2418,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>274</v>
       </c>
@@ -2423,7 +2426,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>276</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>180</v>
       </c>
@@ -2439,7 +2442,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>278</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>280</v>
       </c>
@@ -2455,7 +2458,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>283</v>
       </c>
@@ -2463,7 +2466,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>285</v>
       </c>
@@ -2474,7 +2477,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>287</v>
       </c>
@@ -2482,7 +2485,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>290</v>
       </c>
@@ -2490,7 +2493,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>291</v>
       </c>
@@ -2498,7 +2501,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>293</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>295</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>297</v>
       </c>
@@ -2522,7 +2525,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>299</v>
       </c>
@@ -2530,7 +2533,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>301</v>
       </c>
@@ -2538,7 +2541,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>303</v>
       </c>
@@ -2546,12 +2549,17 @@
         <v>304</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>306</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added editors through b
</commit_message>
<xml_diff>
--- a/authorities_to_be_added.xlsx
+++ b/authorities_to_be_added.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="69" documentId="5_{6FAD9413-535E-401B-86AD-C6AB2D41F333}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A95840D4-BFF9-471E-873E-6F573FBE3BE6}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="5_{6FAD9413-535E-401B-86AD-C6AB2D41F333}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{49100937-5105-4A92-8195-E238CFD3FBD7}"/>
   <bookViews>
     <workbookView xWindow="6108" yWindow="3744" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="427">
   <si>
     <t>Name</t>
   </si>
@@ -1139,6 +1139,168 @@
   </si>
   <si>
     <t>http://viaf.org/viaf/61889969</t>
+  </si>
+  <si>
+    <t>Breigleb, Johann Christian</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/35210135</t>
+  </si>
+  <si>
+    <t>Brix, Ernst Julius</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/35210587</t>
+  </si>
+  <si>
+    <t>Brockhard, Michael</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/191166404</t>
+  </si>
+  <si>
+    <t>Brodribb, William Jackson</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/76716202</t>
+  </si>
+  <si>
+    <t>Church, Alfred John</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/45233331</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/164447798</t>
+  </si>
+  <si>
+    <t>Brohm, Karl Friedr. Aug.</t>
+  </si>
+  <si>
+    <t>Brossaeus, C.</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/59079671</t>
+  </si>
+  <si>
+    <t>Browning, Oscar</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/130145857831723020397</t>
+  </si>
+  <si>
+    <t>Bruder, Carl Hermann</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/18273247</t>
+  </si>
+  <si>
+    <t>Brunck, Richard Francois-Phillipe</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/82656304</t>
+  </si>
+  <si>
+    <t>Bruno, Agostino</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/22515703</t>
+  </si>
+  <si>
+    <t>Bruns, Paul Jakob</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/17983318</t>
+  </si>
+  <si>
+    <t>Bryce, Archilbald Hamilton</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/89610712</t>
+  </si>
+  <si>
+    <t>Buckley, Theodore Alors</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/45879798</t>
+  </si>
+  <si>
+    <t>Budai, Ezsaias</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/39386168</t>
+  </si>
+  <si>
+    <t>Buenemann, Johann Ludolf</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/780439</t>
+  </si>
+  <si>
+    <t>Burman, Kasper</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/88788037</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/47055143</t>
+  </si>
+  <si>
+    <t>Reiske, Johann Jacob</t>
+  </si>
+  <si>
+    <t>Franz, Johann Georg Friedrich</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/12619940</t>
+  </si>
+  <si>
+    <t>Matthiae, F.C.</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/69692810</t>
+  </si>
+  <si>
+    <t>Heinsius, Daniel</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/56635500</t>
+  </si>
+  <si>
+    <t>Heinsius, Nicolaas</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/95302161</t>
+  </si>
+  <si>
+    <t>Ciofano, Ercole</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/45056369</t>
+  </si>
+  <si>
+    <t>Moltzer, Jakob</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/56633987</t>
+  </si>
+  <si>
+    <t>Burnouf, Emile</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/56629753</t>
+  </si>
+  <si>
+    <t>Burton, Edward</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/75042825</t>
+  </si>
+  <si>
+    <t>Buttmann, Phillip</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/39611820</t>
   </si>
 </sst>
 </file>
@@ -1504,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E187"/>
+  <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B187" sqref="B187"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="A216" sqref="A216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2157,7 +2319,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="33.6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>160</v>
       </c>
@@ -3014,6 +3176,230 @@
       </c>
       <c r="B187" s="3" t="s">
         <v>372</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B198" s="6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added work authorities for Statius, etc.
</commit_message>
<xml_diff>
--- a/authorities_to_be_added.xlsx
+++ b/authorities_to_be_added.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="130" documentId="5_{6FAD9413-535E-401B-86AD-C6AB2D41F333}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{49100937-5105-4A92-8195-E238CFD3FBD7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FF2E59-CC0A-45E8-BB5B-C44A209677DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6108" yWindow="3744" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6110" yWindow="3740" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="428">
   <si>
     <t>Name</t>
   </si>
@@ -1301,6 +1301,9 @@
   </si>
   <si>
     <t>http://viaf.org/viaf/39611820</t>
+  </si>
+  <si>
+    <t>Messala Corvinus's De Augusti Progenie???</t>
   </si>
 </sst>
 </file>
@@ -1666,20 +1669,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E215"/>
+  <dimension ref="A1:E216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
       <selection activeCell="A216" sqref="A216"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="84.44140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="44.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="84.453125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1695,7 +1698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1703,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1727,7 +1730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1735,7 +1738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1743,7 +1746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1751,7 +1754,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1759,7 +1762,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1799,7 +1802,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -1839,7 +1842,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>70</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>74</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -1863,7 +1866,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -1879,7 +1882,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>82</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>86</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
@@ -1903,7 +1906,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>90</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -1927,7 +1930,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>96</v>
       </c>
@@ -1935,7 +1938,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>98</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -1959,7 +1962,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1967,7 +1970,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -1983,7 +1986,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
@@ -2007,7 +2010,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
@@ -2015,7 +2018,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -2023,7 +2026,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
@@ -2031,7 +2034,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -2039,7 +2042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>66</v>
       </c>
@@ -2047,7 +2050,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>32</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
@@ -2071,7 +2074,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>84</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
@@ -2087,7 +2090,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>108</v>
       </c>
@@ -2119,7 +2122,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>110</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>114</v>
       </c>
@@ -2143,7 +2146,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>116</v>
       </c>
@@ -2151,7 +2154,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>118</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
@@ -2175,7 +2178,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>124</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
@@ -2191,7 +2194,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>129</v>
       </c>
@@ -2199,7 +2202,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>132</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>135</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>138</v>
       </c>
@@ -2239,7 +2242,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>140</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
@@ -2255,7 +2258,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>144</v>
       </c>
@@ -2263,7 +2266,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>153</v>
       </c>
@@ -2271,7 +2274,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>147</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>149</v>
       </c>
@@ -2287,7 +2290,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>151</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>154</v>
       </c>
@@ -2303,7 +2306,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>156</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>158</v>
       </c>
@@ -2319,7 +2322,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>160</v>
       </c>
@@ -2327,7 +2330,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>162</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>164</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>166</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>168</v>
       </c>
@@ -2359,7 +2362,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>170</v>
       </c>
@@ -2367,7 +2370,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>172</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>174</v>
       </c>
@@ -2383,7 +2386,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>176</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>178</v>
       </c>
@@ -2399,7 +2402,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>180</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>182</v>
       </c>
@@ -2415,7 +2418,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>184</v>
       </c>
@@ -2423,7 +2426,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>186</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>188</v>
       </c>
@@ -2439,7 +2442,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>190</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>192</v>
       </c>
@@ -2455,7 +2458,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>194</v>
       </c>
@@ -2463,7 +2466,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>196</v>
       </c>
@@ -2471,7 +2474,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>198</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>200</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>202</v>
       </c>
@@ -2495,7 +2498,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>204</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>206</v>
       </c>
@@ -2511,7 +2514,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>208</v>
       </c>
@@ -2519,7 +2522,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>210</v>
       </c>
@@ -2527,7 +2530,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>212</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>214</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>216</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>218</v>
       </c>
@@ -2559,7 +2562,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>220</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>222</v>
       </c>
@@ -2575,7 +2578,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>224</v>
       </c>
@@ -2583,7 +2586,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>226</v>
       </c>
@@ -2591,7 +2594,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>228</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>230</v>
       </c>
@@ -2607,7 +2610,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>232</v>
       </c>
@@ -2615,7 +2618,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>234</v>
       </c>
@@ -2623,7 +2626,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>236</v>
       </c>
@@ -2631,7 +2634,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>238</v>
       </c>
@@ -2639,7 +2642,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>240</v>
       </c>
@@ -2647,7 +2650,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>242</v>
       </c>
@@ -2655,7 +2658,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>244</v>
       </c>
@@ -2663,7 +2666,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>246</v>
       </c>
@@ -2671,7 +2674,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>248</v>
       </c>
@@ -2679,7 +2682,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>250</v>
       </c>
@@ -2687,7 +2690,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>257</v>
       </c>
@@ -2695,7 +2698,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>253</v>
       </c>
@@ -2703,7 +2706,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>255</v>
       </c>
@@ -2711,7 +2714,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>258</v>
       </c>
@@ -2719,7 +2722,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>260</v>
       </c>
@@ -2727,7 +2730,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>262</v>
       </c>
@@ -2735,7 +2738,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>263</v>
       </c>
@@ -2743,7 +2746,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>266</v>
       </c>
@@ -2751,7 +2754,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>268</v>
       </c>
@@ -2759,7 +2762,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>270</v>
       </c>
@@ -2767,7 +2770,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>272</v>
       </c>
@@ -2775,7 +2778,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>274</v>
       </c>
@@ -2783,7 +2786,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>276</v>
       </c>
@@ -2791,7 +2794,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>180</v>
       </c>
@@ -2799,7 +2802,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>278</v>
       </c>
@@ -2807,7 +2810,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>280</v>
       </c>
@@ -2815,7 +2818,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>283</v>
       </c>
@@ -2823,7 +2826,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>285</v>
       </c>
@@ -2834,7 +2837,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>287</v>
       </c>
@@ -2842,7 +2845,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>290</v>
       </c>
@@ -2850,7 +2853,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>291</v>
       </c>
@@ -2858,7 +2861,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>293</v>
       </c>
@@ -2866,7 +2869,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>295</v>
       </c>
@@ -2874,7 +2877,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>297</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>299</v>
       </c>
@@ -2890,7 +2893,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>301</v>
       </c>
@@ -2898,7 +2901,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>303</v>
       </c>
@@ -2906,7 +2909,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>305</v>
       </c>
@@ -2914,7 +2917,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>307</v>
       </c>
@@ -2922,7 +2925,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>309</v>
       </c>
@@ -2930,7 +2933,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>311</v>
       </c>
@@ -2938,7 +2941,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>313</v>
       </c>
@@ -2946,7 +2949,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>315</v>
       </c>
@@ -2954,7 +2957,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>317</v>
       </c>
@@ -2962,7 +2965,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>319</v>
       </c>
@@ -2970,7 +2973,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>321</v>
       </c>
@@ -2978,7 +2981,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>323</v>
       </c>
@@ -2986,7 +2989,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>325</v>
       </c>
@@ -2994,7 +2997,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>327</v>
       </c>
@@ -3002,7 +3005,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>329</v>
       </c>
@@ -3010,7 +3013,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>331</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>333</v>
       </c>
@@ -3026,7 +3029,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>335</v>
       </c>
@@ -3034,7 +3037,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>337</v>
       </c>
@@ -3042,7 +3045,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>339</v>
       </c>
@@ -3050,7 +3053,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>341</v>
       </c>
@@ -3058,7 +3061,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>343</v>
       </c>
@@ -3066,7 +3069,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>345</v>
       </c>
@@ -3074,7 +3077,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>347</v>
       </c>
@@ -3082,7 +3085,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>349</v>
       </c>
@@ -3090,7 +3093,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>351</v>
       </c>
@@ -3098,7 +3101,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>353</v>
       </c>
@@ -3106,7 +3109,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>355</v>
       </c>
@@ -3114,7 +3117,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>357</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>359</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>361</v>
       </c>
@@ -3138,7 +3141,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>363</v>
       </c>
@@ -3146,7 +3149,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>365</v>
       </c>
@@ -3154,7 +3157,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>367</v>
       </c>
@@ -3162,7 +3165,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>369</v>
       </c>
@@ -3170,7 +3173,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>371</v>
       </c>
@@ -3178,7 +3181,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>373</v>
       </c>
@@ -3186,7 +3189,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>375</v>
       </c>
@@ -3194,7 +3197,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>377</v>
       </c>
@@ -3202,7 +3205,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>379</v>
       </c>
@@ -3210,7 +3213,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>381</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>384</v>
       </c>
@@ -3226,7 +3229,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>385</v>
       </c>
@@ -3234,7 +3237,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>387</v>
       </c>
@@ -3242,7 +3245,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>389</v>
       </c>
@@ -3250,7 +3253,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>391</v>
       </c>
@@ -3258,7 +3261,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>393</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>395</v>
       </c>
@@ -3274,7 +3277,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>397</v>
       </c>
@@ -3282,7 +3285,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>399</v>
       </c>
@@ -3290,7 +3293,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>401</v>
       </c>
@@ -3298,7 +3301,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>403</v>
       </c>
@@ -3306,7 +3309,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>405</v>
       </c>
@@ -3314,7 +3317,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>408</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>409</v>
       </c>
@@ -3330,7 +3333,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>192</v>
       </c>
@@ -3338,7 +3341,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>411</v>
       </c>
@@ -3346,7 +3349,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>413</v>
       </c>
@@ -3354,7 +3357,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>415</v>
       </c>
@@ -3362,7 +3365,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>417</v>
       </c>
@@ -3370,7 +3373,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>419</v>
       </c>
@@ -3378,7 +3381,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>421</v>
       </c>
@@ -3386,7 +3389,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>423</v>
       </c>
@@ -3394,12 +3397,17 @@
         <v>424</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>425</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>426</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited through row 700
</commit_message>
<xml_diff>
--- a/authorities_to_be_added.xlsx
+++ b/authorities_to_be_added.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="182" documentId="5_{AE778009-62E1-45E1-805C-3F3CA5DB8896}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{480D6A3D-3F0B-4BC3-8EF8-21C51645754A}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="5_{AE778009-62E1-45E1-805C-3F3CA5DB8896}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{DE48F3CE-2035-444D-84BA-57A332C57DD8}"/>
   <bookViews>
-    <workbookView xWindow="6108" yWindow="3744" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="627">
   <si>
     <t>Name</t>
   </si>
@@ -1711,12 +1711,6 @@
     <t>http://viaf.org/viaf/44351611</t>
   </si>
   <si>
-    <t>Davies, John</t>
-  </si>
-  <si>
-    <t>http://viaf.org/viaf/65186822</t>
-  </si>
-  <si>
     <t>Crevier, J.B.L.</t>
   </si>
   <si>
@@ -1805,6 +1799,108 @@
   </si>
   <si>
     <t>Mai, Angelo</t>
+  </si>
+  <si>
+    <t>Dummler, Ernst</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/2552226</t>
+  </si>
+  <si>
+    <t>Duntzer, Heinrich</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/46844264</t>
+  </si>
+  <si>
+    <t>Desprez, Louis</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/78823988</t>
+  </si>
+  <si>
+    <t>Gottschling, Caspar</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/71723197</t>
+  </si>
+  <si>
+    <t>Daehne, Johann Christoph</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/273408152</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/74191242</t>
+  </si>
+  <si>
+    <t>Dahl, Johann Christian Wilhelm</t>
+  </si>
+  <si>
+    <t>Damm, Christian T.</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/69671059</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/6645</t>
+  </si>
+  <si>
+    <t>D'Andilly, Robert Arnaud</t>
+  </si>
+  <si>
+    <t>Gude, Marquard</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/59865177</t>
+  </si>
+  <si>
+    <t>Daniel, Hermann Adelbert</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/47102624</t>
+  </si>
+  <si>
+    <t>Danz, Jo. Traug, Lebr.</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/45043944</t>
+  </si>
+  <si>
+    <t>Daremberg, C.</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/84795155</t>
+  </si>
+  <si>
+    <t>Davidson, Joseph</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/4149155286674687180000</t>
+  </si>
+  <si>
+    <t>Davies, James</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/21302436</t>
+  </si>
+  <si>
+    <t>Bohier, Nicolas</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/12481096</t>
+  </si>
+  <si>
+    <t>Turnebe, Adrien</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/7445187</t>
+  </si>
+  <si>
+    <t>Fabre, Pierre</t>
+  </si>
+  <si>
+    <t>http://viaf.org/viaf/73851967</t>
   </si>
 </sst>
 </file>
@@ -2170,10 +2266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E301"/>
+  <dimension ref="A1:E317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
-      <selection activeCell="A302" sqref="A302"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="A318" sqref="A318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4551,48 +4647,176 @@
         <v>586</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="B297" s="3" t="s">
+      <c r="B297" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="1" t="s">
+      <c r="B298" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="B298" s="1" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="299" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>590</v>
       </c>
-      <c r="B299" s="3" t="s">
+      <c r="B299" s="4" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>592</v>
       </c>
-      <c r="B300" s="4" t="s">
-        <v>593</v>
+      <c r="B300" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B301" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="B301" s="3" t="s">
-        <v>308</v>
+    </row>
+    <row r="302" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A302" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B302" s="3" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A303" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B303" s="3" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A304" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B304" s="3" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A305" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B305" s="3" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A306" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B306" s="3" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A307" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B307" s="3" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A308" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B308" s="3" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A309" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="B309" s="3" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A310" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B310" s="3" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A311" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B311" s="3" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A312" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B312" s="3" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A313" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="B313" s="3" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A314" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B314" s="3" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A315" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B315" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A316" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B316" s="3" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" ht="16.8" x14ac:dyDescent="0.25">
+      <c r="A317" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B317" s="3" t="s">
+        <v>626</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B50">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B50">
     <sortCondition ref="A28"/>
   </sortState>
   <hyperlinks>
@@ -4604,7 +4828,7 @@
     <hyperlink ref="B143" r:id="rId6" xr:uid="{233AB2B0-17DD-49C2-8AF8-74E1B2A40943}"/>
     <hyperlink ref="B144" r:id="rId7" display="http://www.worldcat.org/identities/np-bolchesi, eduard/" xr:uid="{2925A39F-7DFA-4B40-AAA7-04557788DBDF}"/>
     <hyperlink ref="B146" r:id="rId8" xr:uid="{702207DE-56C9-462D-B3BB-ACA04353DB56}"/>
-    <hyperlink ref="B300" r:id="rId9" xr:uid="{BE116454-668C-4656-8D25-0E4297831C21}"/>
+    <hyperlink ref="B299" r:id="rId9" xr:uid="{BE116454-668C-4656-8D25-0E4297831C21}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>

</xml_diff>